<commit_message>
I did so much I forgot what i last commited oops
</commit_message>
<xml_diff>
--- a/Complex Retirement.xlsx
+++ b/Complex Retirement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marconunez/Documents/Financial Modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16729286-BA8E-2148-8321-F3C9F16CA774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CB7CE7-97B5-C74E-8073-A4A6FBFD2F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{6C2D7166-DF05-E94D-BB83-DCCAD6141E39}"/>
   </bookViews>
@@ -3877,7 +3877,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>